<commit_message>
Generate Report for Handoff
</commit_message>
<xml_diff>
--- a/ol-handback/OpenLocalizationOrg/PowerShell-Docs/master/localization-status.xlsx
+++ b/ol-handback/OpenLocalizationOrg/PowerShell-Docs/master/localization-status.xlsx
@@ -2599,7 +2599,7 @@
     <t>Handoff transform failed</t>
   </si>
   <si>
-    <t>2017-08-14 15:46:53</t>
+    <t>2017-08-14 16:46:39</t>
   </si>
   <si>
     <t>Source File Name</t>
@@ -4081,7 +4081,7 @@
     <t>ecmaxml</t>
   </si>
   <si>
-    <t>2017-08-14 15:46:43</t>
+    <t>2017-08-14 16:46:31</t>
   </si>
   <si>
     <t>Internal Server Error

</xml_diff>